<commit_message>
generalized id tracking so that order doesnt matter
</commit_message>
<xml_diff>
--- a/datasets/video-data.xlsx
+++ b/datasets/video-data.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="movie-data" sheetId="1" r:id="rId1"/>
     <sheet name="urls" sheetId="3" r:id="rId2"/>
-    <sheet name="bubble-data" sheetId="4" r:id="rId3"/>
-    <sheet name="bubble-scatter-data" sheetId="2" r:id="rId4"/>
+    <sheet name="bubble-scatter-data" sheetId="4" r:id="rId3"/>
+    <sheet name="bubble-data" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="dataset_1a_movies" localSheetId="2">'bubble-data'!$E$2:$I$12</definedName>
-    <definedName name="dataset_1a_movies" localSheetId="3">'bubble-scatter-data'!$B$2:$I$12</definedName>
+    <definedName name="dataset_1a_movies" localSheetId="3">'bubble-data'!#REF!</definedName>
+    <definedName name="dataset_1a_movies" localSheetId="2">'bubble-scatter-data'!$E$2:$I$12</definedName>
     <definedName name="temp" localSheetId="0">'movie-data'!$E$2:$I$7</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -36,7 +36,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="dataset-1a_movies" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="dataset-1a_movies1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="65001" sourceFile="/Users/Luke/Desktop/ac-d3/example-visualizations/datasets/dataset-1a_movies.csv" comma="1">
       <textFields count="7">
         <textField/>
@@ -49,7 +49,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="dataset-1a_movies1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" name="dataset-1a_movies11" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="65001" sourceFile="/Users/Luke/Desktop/ac-d3/example-visualizations/datasets/dataset-1a_movies.csv" comma="1">
       <textFields count="7">
         <textField/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="89">
   <si>
     <t>type</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>m_id</t>
   </si>
   <si>
     <t>Star Wars: The Force Awakens Official Trailer #1 (2015) - Star Wars Movie HD</t>
@@ -370,7 +367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +377,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -474,6 +477,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +498,6 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dataset-1a_movies" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dataset-1a_movies" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -765,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,28 +787,28 @@
   <sheetData>
     <row r="2" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>3</v>
@@ -818,7 +819,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -827,10 +828,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" s="2" t="str">
         <f>CONCATENATE("https://www.youtube.com/watch?v=",F3,G3)</f>
@@ -849,7 +850,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -858,10 +859,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="2" t="str">
         <f t="shared" ref="H4:H30" si="0">CONCATENATE("https://www.youtube.com/watch?v=",F4,G4)</f>
@@ -880,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="2">
         <v>3</v>
@@ -889,10 +890,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -911,7 +912,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="2">
         <v>4</v>
@@ -920,10 +921,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -942,7 +943,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="2">
         <v>5</v>
@@ -951,10 +952,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -973,7 +974,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2">
         <v>6</v>
@@ -1002,7 +1003,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2">
         <v>7</v>
@@ -1031,7 +1032,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2">
         <v>8</v>
@@ -1307,7 +1308,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
@@ -1319,10 +1320,10 @@
         <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1338,10 +1339,10 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="2">
         <v>20</v>
@@ -1350,10 +1351,10 @@
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1369,10 +1370,10 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D23" s="2">
         <v>21</v>
@@ -1381,10 +1382,10 @@
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1401,7 +1402,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>23</v>
@@ -1413,10 +1414,10 @@
         <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1432,7 +1433,7 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>25</v>
@@ -1444,10 +1445,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1463,7 +1464,7 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>27</v>
@@ -1475,10 +1476,10 @@
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1494,7 +1495,7 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>29</v>
@@ -1506,10 +1507,10 @@
         <v>1</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1525,7 +1526,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>30</v>
@@ -1537,10 +1538,10 @@
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1556,7 +1557,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>31</v>
@@ -1568,10 +1569,10 @@
         <v>1</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H29" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1587,7 +1588,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>32</v>
@@ -1599,10 +1600,10 @@
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H30" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1705,7 +1706,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1720,34 +1721,34 @@
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="11"/>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E5" s="3">
         <v>37873697</v>
@@ -1755,23 +1756,23 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="C9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -1806,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1822,12 +1823,12 @@
   <sheetData>
     <row r="2" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1850,12 +1851,12 @@
       <c r="B3" s="2">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B3,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C3" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Avatar</v>
       </c>
-      <c r="D3" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B3,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D3" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/5PSNL1qE6VY?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E3" s="2">
@@ -1878,12 +1879,12 @@
       <c r="B4" s="2">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B4,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C4" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v xml:space="preserve">Star Wars: The Force Awakens Official Trailer </v>
       </c>
-      <c r="D4" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B4,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D4" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/gAUxw4umkdY?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E4" s="2">
@@ -1906,12 +1907,12 @@
       <c r="B5" s="2">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B5,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C5" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Pirates of the Caribbean: At World's End</v>
       </c>
-      <c r="D5" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B5,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D5" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/HKSZtp_OGHY?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E5" s="2">
@@ -1934,12 +1935,12 @@
       <c r="B6" s="2">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B6,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C6" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Spectre</v>
       </c>
-      <c r="D6" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B6,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D6" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/7GqClqvlObY?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E6" s="2">
@@ -1962,12 +1963,12 @@
       <c r="B7" s="2">
         <v>23</v>
       </c>
-      <c r="C7" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B7,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C7" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>The Dark Knight Rises</v>
       </c>
-      <c r="D7" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B7,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D7" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/GokKUqLcvD8?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E7" s="2">
@@ -1990,12 +1991,12 @@
       <c r="B8" s="2">
         <v>24</v>
       </c>
-      <c r="C8" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B8,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C8" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>John Carter</v>
       </c>
-      <c r="D8" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B8,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D8" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/nlvYKl1fjBI?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E8" s="2">
@@ -2018,12 +2019,12 @@
       <c r="B9" s="2">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B9,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C9" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>The Lone Ranger</v>
       </c>
-      <c r="D9" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B9,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D9" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/JjFsNSoDZK8?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E9" s="2">
@@ -2046,12 +2047,12 @@
       <c r="B10" s="2">
         <v>26</v>
       </c>
-      <c r="C10" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B10,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C10" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Tangled</v>
       </c>
-      <c r="D10" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B10,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D10" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/2f516ZLyC6U?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E10" s="2">
@@ -2074,12 +2075,12 @@
       <c r="B11" s="2">
         <v>27</v>
       </c>
-      <c r="C11" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B11,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C11" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Spider-Man 3</v>
       </c>
-      <c r="D11" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B11,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D11" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/MTIP-Ih_GR0?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E11" s="2">
@@ -2102,12 +2103,12 @@
       <c r="B12" s="2">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-data'!$B12,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="C12" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Avengers: Age of Ultron</v>
       </c>
-      <c r="D12" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-data'!$B12,'bubble-data'!$B$3:$B$12,0))</f>
+      <c r="D12" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/tmeOjFno6Do?autoplay=1&amp;enablejsapi=1</v>
       </c>
       <c r="E12" s="2">
@@ -2133,326 +2134,202 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I12"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="65.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7">
-        <v>40165</v>
-      </c>
-      <c r="E3" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H3,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>19</v>
+      </c>
+      <c r="C3" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Avatar</v>
       </c>
-      <c r="F3" s="2">
-        <v>425000000</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2783918982</v>
-      </c>
-      <c r="H3" s="2">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H3,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D3" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/5PSNL1qE6VY?autoplay=1&amp;enablejsapi=1</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E3" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>4223586</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="7">
-        <v>42356</v>
-      </c>
-      <c r="E4" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H4,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>20</v>
+      </c>
+      <c r="C4" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v xml:space="preserve">Star Wars: The Force Awakens Official Trailer </v>
       </c>
-      <c r="F4" s="2">
-        <v>306000000</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2058662225</v>
-      </c>
-      <c r="H4" s="2">
-        <v>20</v>
-      </c>
-      <c r="I4" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H4,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D4" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/gAUxw4umkdY?autoplay=1&amp;enablejsapi=1</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E4" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>3417742</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7">
-        <v>39226</v>
-      </c>
-      <c r="E5" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H5,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>21</v>
+      </c>
+      <c r="C5" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Pirates of the Caribbean: At World's End</v>
       </c>
-      <c r="F5" s="2">
-        <v>300000000</v>
-      </c>
-      <c r="G5" s="2">
-        <v>963420425</v>
-      </c>
-      <c r="H5" s="2">
-        <v>21</v>
-      </c>
-      <c r="I5" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H5,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D5" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/HKSZtp_OGHY?autoplay=1&amp;enablejsapi=1</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E5" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>882350</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>7</v>
-      </c>
-      <c r="D6" s="7">
-        <v>42314</v>
-      </c>
-      <c r="E6" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H6,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>22</v>
+      </c>
+      <c r="C6" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Spectre</v>
       </c>
-      <c r="F6" s="2">
-        <v>300000000</v>
-      </c>
-      <c r="G6" s="2">
-        <v>879620923</v>
-      </c>
-      <c r="H6" s="2">
-        <v>22</v>
-      </c>
-      <c r="I6" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H6,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D6" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/7GqClqvlObY?autoplay=1&amp;enablejsapi=1</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E6" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>14084581</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7">
-        <v>41110</v>
-      </c>
-      <c r="E7" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H7,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>23</v>
+      </c>
+      <c r="C7" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>The Dark Knight Rises</v>
       </c>
-      <c r="F7" s="2">
-        <v>275000000</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1084439099</v>
-      </c>
-      <c r="H7" s="2">
-        <v>23</v>
-      </c>
-      <c r="I7" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H7,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D7" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/GokKUqLcvD8?autoplay=1&amp;enablejsapi=1</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E7" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>35670361</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7">
-        <v>40977</v>
-      </c>
-      <c r="E8" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H8,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>24</v>
+      </c>
+      <c r="C8" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>John Carter</v>
       </c>
-      <c r="F8" s="2">
-        <v>275000000</v>
-      </c>
-      <c r="G8" s="2">
-        <v>282778100</v>
-      </c>
-      <c r="H8" s="2">
-        <v>24</v>
-      </c>
-      <c r="I8" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H8,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D8" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/nlvYKl1fjBI?autoplay=1&amp;enablejsapi=1</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E8" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>3631219</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2">
-        <v>10</v>
-      </c>
-      <c r="D9" s="7">
-        <v>41457</v>
-      </c>
-      <c r="E9" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H9,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>25</v>
+      </c>
+      <c r="C9" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>The Lone Ranger</v>
       </c>
-      <c r="F9" s="2">
-        <v>275000000</v>
-      </c>
-      <c r="G9" s="2">
-        <v>260002115</v>
-      </c>
-      <c r="H9" s="2">
-        <v>25</v>
-      </c>
-      <c r="I9" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H9,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D9" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/JjFsNSoDZK8?autoplay=1&amp;enablejsapi=1</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E9" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>8186148</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2">
-        <v>8</v>
-      </c>
-      <c r="D10" s="7">
-        <v>40506</v>
-      </c>
-      <c r="E10" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H10,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>26</v>
+      </c>
+      <c r="C10" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Tangled</v>
       </c>
-      <c r="F10" s="2">
-        <v>260000000</v>
-      </c>
-      <c r="G10" s="2">
-        <v>586581936</v>
-      </c>
-      <c r="H10" s="2">
-        <v>26</v>
-      </c>
-      <c r="I10" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H10,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D10" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/2f516ZLyC6U?autoplay=1&amp;enablejsapi=1</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E10" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>4408105</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2">
-        <v>6</v>
-      </c>
-      <c r="D11" s="7">
-        <v>39206</v>
-      </c>
-      <c r="E11" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H11,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>27</v>
+      </c>
+      <c r="C11" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Spider-Man 3</v>
       </c>
-      <c r="F11" s="2">
-        <v>258000000</v>
-      </c>
-      <c r="G11" s="2">
-        <v>890875303</v>
-      </c>
-      <c r="H11" s="2">
-        <v>27</v>
-      </c>
-      <c r="I11" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H11,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D11" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/MTIP-Ih_GR0?autoplay=1&amp;enablejsapi=1</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E11" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>1311286</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="7">
-        <v>42009</v>
-      </c>
-      <c r="E12" s="2" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$H12,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+        <v>28</v>
+      </c>
+      <c r="C12" s="14" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Avengers: Age of Ultron</v>
       </c>
-      <c r="F12" s="2">
-        <v>250000000</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1404705868</v>
-      </c>
-      <c r="H12" s="2">
-        <v>28</v>
-      </c>
-      <c r="I12" s="2" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$H12,'bubble-scatter-data'!$H$3:$H$12,0))</f>
+      <c r="D12" s="14" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>https://www.youtube.com/embed/tmeOjFno6Do?autoplay=1&amp;enablejsapi=1</v>
+      </c>
+      <c r="E12" s="14">
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <v>80560780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added videos to dev-test
</commit_message>
<xml_diff>
--- a/datasets/video-data.xlsx
+++ b/datasets/video-data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luke/Desktop/ac-d3/example-visualizations/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luke/Desktop/ac-d3/AC-D3/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="movie-data" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="88">
   <si>
     <t>type</t>
   </si>
@@ -251,9 +251,6 @@
   </si>
   <si>
     <t>suffixes</t>
-  </si>
-  <si>
-    <t>?autoplay=1&amp;enablejsapi=1</t>
   </si>
   <si>
     <t>videoURL</t>
@@ -465,6 +462,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -477,8 +476,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -787,13 +784,13 @@
   <sheetData>
     <row r="2" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
@@ -805,10 +802,10 @@
         <v>57</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>3</v>
@@ -819,7 +816,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -830,16 +827,14 @@
       <c r="F3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="2" t="str">
         <f>CONCATENATE("https://www.youtube.com/watch?v=",F3,G3)</f>
-        <v>https://www.youtube.com/watch?v=F-eMt3SrfFU?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=F-eMt3SrfFU</v>
       </c>
       <c r="I3" s="2" t="str">
         <f>CONCATENATE("https://www.youtube.com/embed/",F3,G3)</f>
-        <v>https://www.youtube.com/embed/F-eMt3SrfFU?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/F-eMt3SrfFU</v>
       </c>
       <c r="J3" s="2">
         <v>21097531</v>
@@ -850,7 +845,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -861,16 +856,14 @@
       <c r="F4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="2" t="str">
         <f t="shared" ref="H4:H30" si="0">CONCATENATE("https://www.youtube.com/watch?v=",F4,G4)</f>
-        <v>https://www.youtube.com/watch?v=XI4Na5JW1ns?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=XI4Na5JW1ns</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" ref="I4:I30" si="1">CONCATENATE("https://www.youtube.com/embed/",F4,G4)</f>
-        <v>https://www.youtube.com/embed/XI4Na5JW1ns?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/XI4Na5JW1ns</v>
       </c>
       <c r="J4" s="2">
         <v>177639</v>
@@ -881,7 +874,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2">
         <v>3</v>
@@ -892,16 +885,14 @@
       <c r="F5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=nsrOCzUwcjE?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=nsrOCzUwcjE</v>
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/nsrOCzUwcjE?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/nsrOCzUwcjE</v>
       </c>
       <c r="J5" s="2">
         <v>1073553</v>
@@ -912,7 +903,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="2">
         <v>4</v>
@@ -923,16 +914,14 @@
       <c r="F6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=AjCebKn4iic?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=AjCebKn4iic</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/AjCebKn4iic?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/AjCebKn4iic</v>
       </c>
       <c r="J6" s="2">
         <v>1507944</v>
@@ -943,7 +932,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="2">
         <v>5</v>
@@ -954,16 +943,14 @@
       <c r="F7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=DiTECkLZ8HM?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=DiTECkLZ8HM</v>
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/DiTECkLZ8HM?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/DiTECkLZ8HM</v>
       </c>
       <c r="J7" s="2">
         <v>26112988</v>
@@ -974,7 +961,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" s="2">
         <v>6</v>
@@ -1003,7 +990,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2">
         <v>7</v>
@@ -1032,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="2">
         <v>8</v>
@@ -1322,16 +1309,14 @@
       <c r="F21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G21" s="2"/>
       <c r="H21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=5PSNL1qE6VY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=5PSNL1qE6VY</v>
       </c>
       <c r="I21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/5PSNL1qE6VY?autoplay=1&amp;enablejsapi=1</v>
+        <f>CONCATENATE("https://www.youtube.com/embed/",F21,G21)</f>
+        <v>https://www.youtube.com/embed/5PSNL1qE6VY</v>
       </c>
       <c r="J21" s="2">
         <v>4223586</v>
@@ -1342,7 +1327,7 @@
         <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22" s="2">
         <v>20</v>
@@ -1353,16 +1338,14 @@
       <c r="F22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G22" s="2"/>
       <c r="H22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=gAUxw4umkdY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=gAUxw4umkdY</v>
       </c>
       <c r="I22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/gAUxw4umkdY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/gAUxw4umkdY</v>
       </c>
       <c r="J22" s="2">
         <v>3417742</v>
@@ -1373,7 +1356,7 @@
         <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="2">
         <v>21</v>
@@ -1384,16 +1367,14 @@
       <c r="F23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G23" s="2"/>
       <c r="H23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=HKSZtp_OGHY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=HKSZtp_OGHY</v>
       </c>
       <c r="I23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/HKSZtp_OGHY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/HKSZtp_OGHY</v>
       </c>
       <c r="J23" s="2">
         <v>882350</v>
@@ -1416,16 +1397,14 @@
       <c r="F24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G24" s="2"/>
       <c r="H24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=7GqClqvlObY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=7GqClqvlObY</v>
       </c>
       <c r="I24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/7GqClqvlObY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/7GqClqvlObY</v>
       </c>
       <c r="J24" s="2">
         <v>14084581</v>
@@ -1447,16 +1426,14 @@
       <c r="F25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="G25" s="2"/>
       <c r="H25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=GokKUqLcvD8?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=GokKUqLcvD8</v>
       </c>
       <c r="I25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/GokKUqLcvD8?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/GokKUqLcvD8</v>
       </c>
       <c r="J25" s="2">
         <v>35670361</v>
@@ -1464,7 +1441,7 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>27</v>
@@ -1476,18 +1453,16 @@
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G26" s="2"/>
       <c r="H26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=nlvYKl1fjBI?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=nlvYKl1fjBI</v>
       </c>
       <c r="I26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/nlvYKl1fjBI?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/nlvYKl1fjBI</v>
       </c>
       <c r="J26" s="2">
         <v>3631219</v>
@@ -1495,7 +1470,7 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>29</v>
@@ -1507,18 +1482,16 @@
         <v>1</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G27" s="2"/>
       <c r="H27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=JjFsNSoDZK8?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=JjFsNSoDZK8</v>
       </c>
       <c r="I27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/JjFsNSoDZK8?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/JjFsNSoDZK8</v>
       </c>
       <c r="J27" s="2">
         <v>8186148</v>
@@ -1526,7 +1499,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>30</v>
@@ -1538,18 +1511,16 @@
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G28" s="2"/>
       <c r="H28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=2f516ZLyC6U?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=2f516ZLyC6U</v>
       </c>
       <c r="I28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/2f516ZLyC6U?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/2f516ZLyC6U</v>
       </c>
       <c r="J28" s="2">
         <v>4408105</v>
@@ -1557,7 +1528,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>31</v>
@@ -1569,18 +1540,16 @@
         <v>1</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G29" s="2"/>
       <c r="H29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=MTIP-Ih_GR0?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=MTIP-Ih_GR0</v>
       </c>
       <c r="I29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/MTIP-Ih_GR0?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/MTIP-Ih_GR0</v>
       </c>
       <c r="J29" s="2">
         <v>1311286</v>
@@ -1588,7 +1557,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>32</v>
@@ -1600,18 +1569,16 @@
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="G30" s="2"/>
       <c r="H30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.youtube.com/watch?v=tmeOjFno6Do?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/watch?v=tmeOjFno6Do</v>
       </c>
       <c r="I30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.youtube.com/embed/tmeOjFno6Do?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/tmeOjFno6Do</v>
       </c>
       <c r="J30" s="2">
         <v>80560780</v>
@@ -1705,8 +1672,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
-        <v>76</v>
+      <c r="B2" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1719,7 +1686,7 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="11"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="2" t="s">
         <v>46</v>
       </c>
@@ -1731,7 +1698,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="11"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1743,7 +1710,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1755,41 +1722,41 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
-        <v>75</v>
+      <c r="B8" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+      <c r="C9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="9"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1823,12 +1790,12 @@
   <sheetData>
     <row r="2" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1851,13 +1818,13 @@
       <c r="B3" s="2">
         <v>19</v>
       </c>
-      <c r="C3" s="14" t="str">
+      <c r="C3" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Avatar</v>
       </c>
-      <c r="D3" s="14" t="str">
+      <c r="D3" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/5PSNL1qE6VY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/5PSNL1qE6VY</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -1879,13 +1846,13 @@
       <c r="B4" s="2">
         <v>20</v>
       </c>
-      <c r="C4" s="14" t="str">
+      <c r="C4" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v xml:space="preserve">Star Wars: The Force Awakens Official Trailer </v>
       </c>
-      <c r="D4" s="14" t="str">
+      <c r="D4" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/gAUxw4umkdY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/gAUxw4umkdY</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1907,13 +1874,13 @@
       <c r="B5" s="2">
         <v>21</v>
       </c>
-      <c r="C5" s="14" t="str">
+      <c r="C5" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Pirates of the Caribbean: At World's End</v>
       </c>
-      <c r="D5" s="14" t="str">
+      <c r="D5" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/HKSZtp_OGHY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/HKSZtp_OGHY</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -1935,13 +1902,13 @@
       <c r="B6" s="2">
         <v>22</v>
       </c>
-      <c r="C6" s="14" t="str">
+      <c r="C6" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Spectre</v>
       </c>
-      <c r="D6" s="14" t="str">
+      <c r="D6" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/7GqClqvlObY?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/7GqClqvlObY</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -1963,13 +1930,13 @@
       <c r="B7" s="2">
         <v>23</v>
       </c>
-      <c r="C7" s="14" t="str">
+      <c r="C7" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>The Dark Knight Rises</v>
       </c>
-      <c r="D7" s="14" t="str">
+      <c r="D7" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/GokKUqLcvD8?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/GokKUqLcvD8</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
@@ -1991,13 +1958,13 @@
       <c r="B8" s="2">
         <v>24</v>
       </c>
-      <c r="C8" s="14" t="str">
+      <c r="C8" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>John Carter</v>
       </c>
-      <c r="D8" s="14" t="str">
+      <c r="D8" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/nlvYKl1fjBI?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/nlvYKl1fjBI</v>
       </c>
       <c r="E8" s="2">
         <v>7</v>
@@ -2019,13 +1986,13 @@
       <c r="B9" s="2">
         <v>25</v>
       </c>
-      <c r="C9" s="14" t="str">
+      <c r="C9" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>The Lone Ranger</v>
       </c>
-      <c r="D9" s="14" t="str">
+      <c r="D9" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/JjFsNSoDZK8?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/JjFsNSoDZK8</v>
       </c>
       <c r="E9" s="2">
         <v>6</v>
@@ -2047,13 +2014,13 @@
       <c r="B10" s="2">
         <v>26</v>
       </c>
-      <c r="C10" s="14" t="str">
+      <c r="C10" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Tangled</v>
       </c>
-      <c r="D10" s="14" t="str">
+      <c r="D10" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/2f516ZLyC6U?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/2f516ZLyC6U</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
@@ -2075,13 +2042,13 @@
       <c r="B11" s="2">
         <v>27</v>
       </c>
-      <c r="C11" s="14" t="str">
+      <c r="C11" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Spider-Man 3</v>
       </c>
-      <c r="D11" s="14" t="str">
+      <c r="D11" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/MTIP-Ih_GR0?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/MTIP-Ih_GR0</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
@@ -2103,13 +2070,13 @@
       <c r="B12" s="2">
         <v>28</v>
       </c>
-      <c r="C12" s="14" t="str">
+      <c r="C12" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Avengers: Age of Ultron</v>
       </c>
-      <c r="D12" s="14" t="str">
+      <c r="D12" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/tmeOjFno6Do?autoplay=1&amp;enablejsapi=1</v>
+        <v>https://www.youtube.com/embed/tmeOjFno6Do</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
@@ -2136,8 +2103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2150,15 +2117,15 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2166,15 +2133,15 @@
       <c r="B3" s="2">
         <v>19</v>
       </c>
-      <c r="C3" s="14" t="str">
+      <c r="C3" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Avatar</v>
       </c>
-      <c r="D3" s="14" t="str">
+      <c r="D3" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/5PSNL1qE6VY?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E3" s="14">
+        <v>https://www.youtube.com/embed/5PSNL1qE6VY</v>
+      </c>
+      <c r="E3" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>4223586</v>
       </c>
@@ -2183,15 +2150,15 @@
       <c r="B4" s="2">
         <v>20</v>
       </c>
-      <c r="C4" s="14" t="str">
+      <c r="C4" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v xml:space="preserve">Star Wars: The Force Awakens Official Trailer </v>
       </c>
-      <c r="D4" s="14" t="str">
+      <c r="D4" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/gAUxw4umkdY?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E4" s="14">
+        <v>https://www.youtube.com/embed/gAUxw4umkdY</v>
+      </c>
+      <c r="E4" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>3417742</v>
       </c>
@@ -2200,15 +2167,15 @@
       <c r="B5" s="2">
         <v>21</v>
       </c>
-      <c r="C5" s="14" t="str">
+      <c r="C5" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Pirates of the Caribbean: At World's End</v>
       </c>
-      <c r="D5" s="14" t="str">
+      <c r="D5" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/HKSZtp_OGHY?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E5" s="14">
+        <v>https://www.youtube.com/embed/HKSZtp_OGHY</v>
+      </c>
+      <c r="E5" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>882350</v>
       </c>
@@ -2217,15 +2184,15 @@
       <c r="B6" s="2">
         <v>22</v>
       </c>
-      <c r="C6" s="14" t="str">
+      <c r="C6" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Spectre</v>
       </c>
-      <c r="D6" s="14" t="str">
+      <c r="D6" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/7GqClqvlObY?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E6" s="14">
+        <v>https://www.youtube.com/embed/7GqClqvlObY</v>
+      </c>
+      <c r="E6" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>14084581</v>
       </c>
@@ -2234,15 +2201,15 @@
       <c r="B7" s="2">
         <v>23</v>
       </c>
-      <c r="C7" s="14" t="str">
+      <c r="C7" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>The Dark Knight Rises</v>
       </c>
-      <c r="D7" s="14" t="str">
+      <c r="D7" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/GokKUqLcvD8?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E7" s="14">
+        <v>https://www.youtube.com/embed/GokKUqLcvD8</v>
+      </c>
+      <c r="E7" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>35670361</v>
       </c>
@@ -2251,15 +2218,15 @@
       <c r="B8" s="2">
         <v>24</v>
       </c>
-      <c r="C8" s="14" t="str">
+      <c r="C8" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>John Carter</v>
       </c>
-      <c r="D8" s="14" t="str">
+      <c r="D8" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/nlvYKl1fjBI?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E8" s="14">
+        <v>https://www.youtube.com/embed/nlvYKl1fjBI</v>
+      </c>
+      <c r="E8" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>3631219</v>
       </c>
@@ -2268,15 +2235,15 @@
       <c r="B9" s="2">
         <v>25</v>
       </c>
-      <c r="C9" s="14" t="str">
+      <c r="C9" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>The Lone Ranger</v>
       </c>
-      <c r="D9" s="14" t="str">
+      <c r="D9" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/JjFsNSoDZK8?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E9" s="14">
+        <v>https://www.youtube.com/embed/JjFsNSoDZK8</v>
+      </c>
+      <c r="E9" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>8186148</v>
       </c>
@@ -2285,15 +2252,15 @@
       <c r="B10" s="2">
         <v>26</v>
       </c>
-      <c r="C10" s="14" t="str">
+      <c r="C10" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Tangled</v>
       </c>
-      <c r="D10" s="14" t="str">
+      <c r="D10" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/2f516ZLyC6U?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E10" s="14">
+        <v>https://www.youtube.com/embed/2f516ZLyC6U</v>
+      </c>
+      <c r="E10" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>4408105</v>
       </c>
@@ -2302,15 +2269,15 @@
       <c r="B11" s="2">
         <v>27</v>
       </c>
-      <c r="C11" s="14" t="str">
+      <c r="C11" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Spider-Man 3</v>
       </c>
-      <c r="D11" s="14" t="str">
+      <c r="D11" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/MTIP-Ih_GR0?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E11" s="14">
+        <v>https://www.youtube.com/embed/MTIP-Ih_GR0</v>
+      </c>
+      <c r="E11" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>1311286</v>
       </c>
@@ -2319,15 +2286,15 @@
       <c r="B12" s="2">
         <v>28</v>
       </c>
-      <c r="C12" s="14" t="str">
+      <c r="C12" s="10" t="str">
         <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>Avengers: Age of Ultron</v>
       </c>
-      <c r="D12" s="14" t="str">
+      <c r="D12" s="10" t="str">
         <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/tmeOjFno6Do?autoplay=1&amp;enablejsapi=1</v>
-      </c>
-      <c r="E12" s="14">
+        <v>https://www.youtube.com/embed/tmeOjFno6Do</v>
+      </c>
+      <c r="E12" s="10">
         <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
         <v>80560780</v>
       </c>

</xml_diff>

<commit_message>
bubble scatter working. before merge with jacobs code
</commit_message>
<xml_diff>
--- a/datasets/video-data.xlsx
+++ b/datasets/video-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="-4540" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="movie-data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="dataset_1a_movies" localSheetId="3">'bubble-data'!#REF!</definedName>
-    <definedName name="dataset_1a_movies" localSheetId="2">'bubble-scatter-data'!$E$2:$I$12</definedName>
+    <definedName name="dataset_1a_movies" localSheetId="2">'bubble-scatter-data'!$B$2:$J$12</definedName>
     <definedName name="temp" localSheetId="0">'movie-data'!$E$2:$I$7</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t>type</t>
   </si>
@@ -124,18 +124,9 @@
     <t>wordlwideGrossRank</t>
   </si>
   <si>
-    <t>releaseDate</t>
-  </si>
-  <si>
     <t>movieName</t>
   </si>
   <si>
-    <t>productionBudget</t>
-  </si>
-  <si>
-    <t>worldwideGross</t>
-  </si>
-  <si>
     <t>Avatar</t>
   </si>
   <si>
@@ -341,6 +332,18 @@
   </si>
   <si>
     <t>v_id</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -763,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,28 +787,28 @@
   <sheetData>
     <row r="2" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>3</v>
@@ -816,7 +819,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -825,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="str">
@@ -845,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -854,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="str">
@@ -874,7 +877,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5" s="2">
         <v>3</v>
@@ -883,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="str">
@@ -903,7 +906,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D6" s="2">
         <v>4</v>
@@ -912,7 +915,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="str">
@@ -932,7 +935,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D7" s="2">
         <v>5</v>
@@ -941,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="str">
@@ -961,7 +964,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D8" s="2">
         <v>6</v>
@@ -990,7 +993,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D9" s="2">
         <v>7</v>
@@ -1019,7 +1022,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D10" s="2">
         <v>8</v>
@@ -1045,7 +1048,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="2">
@@ -1055,22 +1058,22 @@
         <v>2</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="2">
@@ -1080,22 +1083,22 @@
         <v>2</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="2">
@@ -1105,22 +1108,22 @@
         <v>2</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="2">
@@ -1130,22 +1133,22 @@
         <v>2</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="2">
@@ -1155,22 +1158,22 @@
         <v>2</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="2">
@@ -1180,22 +1183,22 @@
         <v>2</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="2">
@@ -1205,22 +1208,22 @@
         <v>2</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="2">
@@ -1230,22 +1233,22 @@
         <v>2</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="2">
@@ -1255,22 +1258,22 @@
         <v>2</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="2">
@@ -1280,25 +1283,25 @@
         <v>2</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D21" s="2">
         <v>19</v>
@@ -1307,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="str">
@@ -1324,10 +1327,10 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D22" s="2">
         <v>20</v>
@@ -1336,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="str">
@@ -1353,10 +1356,10 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D23" s="2">
         <v>21</v>
@@ -1365,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="str">
@@ -1383,10 +1386,10 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D24" s="2">
         <v>22</v>
@@ -1395,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="str">
@@ -1412,10 +1415,10 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D25" s="2">
         <v>23</v>
@@ -1424,7 +1427,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="str">
@@ -1441,10 +1444,10 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D26" s="2">
         <v>24</v>
@@ -1453,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="str">
@@ -1470,10 +1473,10 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2">
         <v>25</v>
@@ -1482,7 +1485,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="str">
@@ -1499,10 +1502,10 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D28" s="2">
         <v>26</v>
@@ -1511,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="str">
@@ -1528,10 +1531,10 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D29" s="2">
         <v>27</v>
@@ -1540,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="str">
@@ -1557,10 +1560,10 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D30" s="2">
         <v>28</v>
@@ -1569,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="str">
@@ -1673,7 +1676,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1688,34 +1691,34 @@
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="13"/>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="13"/>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="14"/>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E5" s="3">
         <v>37873697</v>
@@ -1723,23 +1726,23 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -1772,325 +1775,363 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I12"/>
+  <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="J2" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D3,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>Avatar</v>
+      </c>
+      <c r="G3" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D3,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>https://www.youtube.com/embed/5PSNL1qE6VY</v>
+      </c>
+      <c r="H3" s="7">
+        <v>40165</v>
+      </c>
+      <c r="I3" s="2">
+        <v>425000000</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2783918982</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="2">
-        <v>19</v>
-      </c>
-      <c r="C3" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>Avatar</v>
-      </c>
-      <c r="D3" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/5PSNL1qE6VY</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7">
-        <v>40165</v>
-      </c>
-      <c r="H3" s="2">
-        <v>425000000</v>
-      </c>
-      <c r="I3" s="2">
-        <v>2783918982</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="2">
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
         <v>20</v>
       </c>
-      <c r="C4" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D4,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v xml:space="preserve">Star Wars: The Force Awakens Official Trailer </v>
       </c>
-      <c r="D4" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+      <c r="G4" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D4,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/gAUxw4umkdY</v>
       </c>
-      <c r="E4" s="2">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="H4" s="7">
         <v>42356</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>306000000</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>2058662225</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
         <v>21</v>
       </c>
-      <c r="C5" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D5,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>Pirates of the Caribbean: At World's End</v>
       </c>
-      <c r="D5" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+      <c r="G5" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D5,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/HKSZtp_OGHY</v>
       </c>
-      <c r="E5" s="2">
+      <c r="H5" s="7">
+        <v>39226</v>
+      </c>
+      <c r="I5" s="2">
+        <v>300000000</v>
+      </c>
+      <c r="J5" s="2">
+        <v>963420425</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D6,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>Spectre</v>
+      </c>
+      <c r="G6" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D6,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>https://www.youtube.com/embed/7GqClqvlObY</v>
+      </c>
+      <c r="H6" s="7">
+        <v>42314</v>
+      </c>
+      <c r="I6" s="2">
+        <v>300000000</v>
+      </c>
+      <c r="J6" s="2">
+        <v>879620923</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D7,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>The Dark Knight Rises</v>
+      </c>
+      <c r="G7" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D7,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>https://www.youtube.com/embed/GokKUqLcvD8</v>
+      </c>
+      <c r="H7" s="7">
+        <v>41110</v>
+      </c>
+      <c r="I7" s="2">
+        <v>275000000</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1084439099</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D8,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>John Carter</v>
+      </c>
+      <c r="G8" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D8,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>https://www.youtube.com/embed/nlvYKl1fjBI</v>
+      </c>
+      <c r="H8" s="7">
+        <v>40977</v>
+      </c>
+      <c r="I8" s="2">
+        <v>275000000</v>
+      </c>
+      <c r="J8" s="2">
+        <v>282778100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D9,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>The Lone Ranger</v>
+      </c>
+      <c r="G9" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D9,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>https://www.youtube.com/embed/JjFsNSoDZK8</v>
+      </c>
+      <c r="H9" s="7">
+        <v>41457</v>
+      </c>
+      <c r="I9" s="2">
+        <v>275000000</v>
+      </c>
+      <c r="J9" s="2">
+        <v>260002115</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D10,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>Tangled</v>
+      </c>
+      <c r="G10" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D10,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>https://www.youtube.com/embed/2f516ZLyC6U</v>
+      </c>
+      <c r="H10" s="7">
+        <v>40506</v>
+      </c>
+      <c r="I10" s="2">
+        <v>260000000</v>
+      </c>
+      <c r="J10" s="2">
+        <v>586581936</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>27</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D11,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>Spider-Man 3</v>
+      </c>
+      <c r="G11" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D11,'bubble-scatter-data'!$D$3:$D$12,0))</f>
+        <v>https://www.youtube.com/embed/MTIP-Ih_GR0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>39206</v>
+      </c>
+      <c r="I11" s="2">
+        <v>258000000</v>
+      </c>
+      <c r="J11" s="2">
+        <v>890875303</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="2">
-        <v>5</v>
-      </c>
-      <c r="G5" s="7">
-        <v>39226</v>
-      </c>
-      <c r="H5" s="2">
-        <v>300000000</v>
-      </c>
-      <c r="I5" s="2">
-        <v>963420425</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="2">
-        <v>22</v>
-      </c>
-      <c r="C6" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>Spectre</v>
-      </c>
-      <c r="D6" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/7GqClqvlObY</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2">
-        <v>7</v>
-      </c>
-      <c r="G6" s="7">
-        <v>42314</v>
-      </c>
-      <c r="H6" s="2">
-        <v>300000000</v>
-      </c>
-      <c r="I6" s="2">
-        <v>879620923</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="2">
-        <v>23</v>
-      </c>
-      <c r="C7" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>The Dark Knight Rises</v>
-      </c>
-      <c r="D7" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/GokKUqLcvD8</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2">
-        <v>4</v>
-      </c>
-      <c r="G7" s="7">
-        <v>41110</v>
-      </c>
-      <c r="H7" s="2">
-        <v>275000000</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1084439099</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="2">
-        <v>24</v>
-      </c>
-      <c r="C8" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>John Carter</v>
-      </c>
-      <c r="D8" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/nlvYKl1fjBI</v>
-      </c>
-      <c r="E8" s="2">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2">
-        <v>9</v>
-      </c>
-      <c r="G8" s="7">
-        <v>40977</v>
-      </c>
-      <c r="H8" s="2">
-        <v>275000000</v>
-      </c>
-      <c r="I8" s="2">
-        <v>282778100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="2">
-        <v>25</v>
-      </c>
-      <c r="C9" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>The Lone Ranger</v>
-      </c>
-      <c r="D9" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/JjFsNSoDZK8</v>
-      </c>
-      <c r="E9" s="2">
-        <v>6</v>
-      </c>
-      <c r="F9" s="2">
-        <v>10</v>
-      </c>
-      <c r="G9" s="7">
-        <v>41457</v>
-      </c>
-      <c r="H9" s="2">
-        <v>275000000</v>
-      </c>
-      <c r="I9" s="2">
-        <v>260002115</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="2">
-        <v>26</v>
-      </c>
-      <c r="C10" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>Tangled</v>
-      </c>
-      <c r="D10" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/2f516ZLyC6U</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
-      </c>
-      <c r="F10" s="2">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7">
-        <v>40506</v>
-      </c>
-      <c r="H10" s="2">
-        <v>260000000</v>
-      </c>
-      <c r="I10" s="2">
-        <v>586581936</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
-        <v>27</v>
-      </c>
-      <c r="C11" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>Spider-Man 3</v>
-      </c>
-      <c r="D11" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
-        <v>https://www.youtube.com/embed/MTIP-Ih_GR0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>9</v>
-      </c>
-      <c r="F11" s="2">
-        <v>6</v>
-      </c>
-      <c r="G11" s="7">
-        <v>39206</v>
-      </c>
-      <c r="H11" s="2">
-        <v>258000000</v>
-      </c>
-      <c r="I11" s="2">
-        <v>890875303</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="2">
+      <c r="D12" s="2">
         <v>28</v>
       </c>
-      <c r="C12" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+      <c r="E12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10" t="str">
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D12,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>Avengers: Age of Ultron</v>
       </c>
-      <c r="D12" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+      <c r="G12" s="10" t="str">
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D12,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/tmeOjFno6Do</v>
       </c>
-      <c r="E12" s="2">
-        <v>10</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="H12" s="7">
         <v>42009</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>250000000</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>1404705868</v>
       </c>
     </row>
@@ -2117,13 +2158,13 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>3</v>
@@ -2134,15 +2175,15 @@
         <v>19</v>
       </c>
       <c r="C3" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D3,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>Avatar</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D3,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/5PSNL1qE6VY</v>
       </c>
       <c r="E3" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B3,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D3,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>4223586</v>
       </c>
     </row>
@@ -2151,15 +2192,15 @@
         <v>20</v>
       </c>
       <c r="C4" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D4,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v xml:space="preserve">Star Wars: The Force Awakens Official Trailer </v>
       </c>
       <c r="D4" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D4,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/gAUxw4umkdY</v>
       </c>
       <c r="E4" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B4,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D4,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>3417742</v>
       </c>
     </row>
@@ -2168,15 +2209,15 @@
         <v>21</v>
       </c>
       <c r="C5" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D5,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>Pirates of the Caribbean: At World's End</v>
       </c>
       <c r="D5" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D5,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/HKSZtp_OGHY</v>
       </c>
       <c r="E5" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B5,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D5,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>882350</v>
       </c>
     </row>
@@ -2185,15 +2226,15 @@
         <v>22</v>
       </c>
       <c r="C6" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D6,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>Spectre</v>
       </c>
       <c r="D6" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D6,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/7GqClqvlObY</v>
       </c>
       <c r="E6" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B6,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D6,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>14084581</v>
       </c>
     </row>
@@ -2202,15 +2243,15 @@
         <v>23</v>
       </c>
       <c r="C7" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D7,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>The Dark Knight Rises</v>
       </c>
       <c r="D7" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D7,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/GokKUqLcvD8</v>
       </c>
       <c r="E7" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B7,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D7,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>35670361</v>
       </c>
     </row>
@@ -2219,15 +2260,15 @@
         <v>24</v>
       </c>
       <c r="C8" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D8,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>John Carter</v>
       </c>
       <c r="D8" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D8,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/nlvYKl1fjBI</v>
       </c>
       <c r="E8" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B8,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D8,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>3631219</v>
       </c>
     </row>
@@ -2236,15 +2277,15 @@
         <v>25</v>
       </c>
       <c r="C9" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D9,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>The Lone Ranger</v>
       </c>
       <c r="D9" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D9,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/JjFsNSoDZK8</v>
       </c>
       <c r="E9" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B9,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D9,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>8186148</v>
       </c>
     </row>
@@ -2253,15 +2294,15 @@
         <v>26</v>
       </c>
       <c r="C10" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D10,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>Tangled</v>
       </c>
       <c r="D10" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D10,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/2f516ZLyC6U</v>
       </c>
       <c r="E10" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B10,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D10,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>4408105</v>
       </c>
     </row>
@@ -2270,15 +2311,15 @@
         <v>27</v>
       </c>
       <c r="C11" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D11,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>Spider-Man 3</v>
       </c>
       <c r="D11" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D11,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/MTIP-Ih_GR0</v>
       </c>
       <c r="E11" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B11,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D11,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>1311286</v>
       </c>
     </row>
@@ -2287,15 +2328,15 @@
         <v>28</v>
       </c>
       <c r="C12" s="10" t="str">
-        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$C$21:$C$31,MATCH('bubble-scatter-data'!$D12,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>Avengers: Age of Ultron</v>
       </c>
       <c r="D12" s="10" t="str">
-        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$I$21:$I$31,MATCH('bubble-scatter-data'!$D12,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>https://www.youtube.com/embed/tmeOjFno6Do</v>
       </c>
       <c r="E12" s="10">
-        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$B12,'bubble-scatter-data'!$B$3:$B$12,0))</f>
+        <f>INDEX('movie-data'!$J$21:$J$31,MATCH('bubble-scatter-data'!$D12,'bubble-scatter-data'!$D$3:$D$12,0))</f>
         <v>80560780</v>
       </c>
     </row>

</xml_diff>